<commit_message>
ng: add lagos forms
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/Nigeria/Oct 2023/ng_oncho_oem_1_site_202310.xlsx
+++ b/ONCHO/OEM/Nigeria/Oct 2023/ng_oncho_oem_1_site_202310.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\ONCHO\OEM\Nigeria\Oct 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50520AF-6782-41F0-80BC-FBBB72C4C664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B083BD-6566-43D7-8DEF-773FC4292512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,10 +620,10 @@
     <t>PEDRO/BANKOLE STREET</t>
   </si>
   <si>
-    <t>ng_oncho_oem_1_site_202310</t>
-  </si>
-  <si>
-    <t>(2023 Oct) - 1. Site Form (Lagos)</t>
+    <t>ng_oncho_oem_1_site_202310_lagos</t>
+  </si>
+  <si>
+    <t>(2023 Oct) - Lagos - 1. Site Form</t>
   </si>
 </sst>
 </file>

</xml_diff>